<commit_message>
first version auto logging of transactions
</commit_message>
<xml_diff>
--- a/My Monthly Budgeting.xlsx
+++ b/My Monthly Budgeting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11122"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7622F179-7A89-3E40-B46E-F5C8370F6E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4053E09-FE1D-334D-BEA5-D7BA6554FAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,8 +37,10 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={1F6482E2-E90C-3A49-93EB-99F21FF6AC85}</author>
+    <author>tc={8B57B6A9-8B6A-B749-8C90-A57E13FBAE58}</author>
     <author>Author</author>
     <author>tc={DDAC9636-E59B-F14B-AA15-13D2CA4ABE00}</author>
+    <author>tc={DBA57A08-AA3B-6145-B7E0-D7C7CDF226A9}</author>
   </authors>
   <commentList>
     <comment ref="V15" authorId="0" shapeId="0" xr:uid="{1F6482E2-E90C-3A49-93EB-99F21FF6AC85}">
@@ -49,7 +51,16 @@
     Ariel's wedding</t>
       </text>
     </comment>
-    <comment ref="T19" authorId="1" shapeId="0" xr:uid="{5611FD8F-9265-1F40-AD0B-D488FC8F6B03}">
+    <comment ref="AR15" authorId="1" shapeId="0" xr:uid="{8B57B6A9-8B6A-B749-8C90-A57E13FBAE58}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    trip to netanya
+</t>
+      </text>
+    </comment>
+    <comment ref="T19" authorId="2" shapeId="0" xr:uid="{5611FD8F-9265-1F40-AD0B-D488FC8F6B03}">
       <text>
         <r>
           <rPr>
@@ -73,12 +84,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="S20" authorId="2" shapeId="0" xr:uid="{DDAC9636-E59B-F14B-AA15-13D2CA4ABE00}">
+    <comment ref="S20" authorId="3" shapeId="0" xr:uid="{DDAC9636-E59B-F14B-AA15-13D2CA4ABE00}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     haircut</t>
+      </text>
+    </comment>
+    <comment ref="AT20" authorId="4" shapeId="0" xr:uid="{DBA57A08-AA3B-6145-B7E0-D7C7CDF226A9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    gift to bati and new pants(Temu)</t>
       </text>
     </comment>
   </commentList>
@@ -3608,6 +3627,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4628,8 +4651,15 @@
   <threadedComment ref="V15" dT="2026-01-12T19:18:52.69" personId="{00000000-0000-0000-0000-000000000000}" id="{1F6482E2-E90C-3A49-93EB-99F21FF6AC85}">
     <text>Ariel's wedding</text>
   </threadedComment>
+  <threadedComment ref="AR15" dT="2026-02-01T09:55:16.57" personId="{00000000-0000-0000-0000-000000000000}" id="{8B57B6A9-8B6A-B749-8C90-A57E13FBAE58}">
+    <text xml:space="preserve">trip to netanya
+</text>
+  </threadedComment>
   <threadedComment ref="S20" dT="2026-01-12T19:19:06.47" personId="{00000000-0000-0000-0000-000000000000}" id="{DDAC9636-E59B-F14B-AA15-13D2CA4ABE00}">
     <text>haircut</text>
+  </threadedComment>
+  <threadedComment ref="AT20" dT="2026-02-01T09:55:33.63" personId="{00000000-0000-0000-0000-000000000000}" id="{DBA57A08-AA3B-6145-B7E0-D7C7CDF226A9}">
+    <text>gift to bati and new pants(Temu)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -18551,8 +18581,8 @@
   </sheetPr>
   <dimension ref="A1:FX65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AJ20" sqref="AJ20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -21127,10 +21157,13 @@
       <c r="AO15" s="24"/>
       <c r="AP15" s="24"/>
       <c r="AQ15" s="24"/>
-      <c r="AR15" s="24"/>
+      <c r="AR15" s="24">
+        <f>SUM(44,100,24,77)</f>
+        <v>245</v>
+      </c>
       <c r="AS15" s="24">
-        <f t="shared" ref="AS15:AS20" si="4">SUM(AL15:AR15)</f>
-        <v>0</v>
+        <f t="shared" ref="AS15:AS19" si="4">SUM(AL15:AR15)</f>
+        <v>245</v>
       </c>
       <c r="AT15" s="24"/>
       <c r="AU15" s="24"/>
@@ -21759,14 +21792,18 @@
       </c>
       <c r="AL18" s="28"/>
       <c r="AM18" s="28"/>
-      <c r="AN18" s="28"/>
+      <c r="AN18" s="28">
+        <v>35</v>
+      </c>
       <c r="AO18" s="28"/>
-      <c r="AP18" s="28"/>
+      <c r="AP18" s="28">
+        <v>191</v>
+      </c>
       <c r="AQ18" s="28"/>
       <c r="AR18" s="28"/>
       <c r="AS18" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>SUM(AL18:AQ18)</f>
+        <v>226</v>
       </c>
       <c r="AT18" s="28"/>
       <c r="AU18" s="28"/>
@@ -22223,14 +22260,21 @@
       <c r="AM19" s="29"/>
       <c r="AN19" s="29"/>
       <c r="AO19" s="29"/>
-      <c r="AP19" s="29"/>
-      <c r="AQ19" s="29"/>
+      <c r="AP19" s="29">
+        <v>45</v>
+      </c>
+      <c r="AQ19" s="29">
+        <f>SUM(79,23)</f>
+        <v>102</v>
+      </c>
       <c r="AR19" s="29"/>
       <c r="AS19" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AT19" s="29"/>
+        <v>147</v>
+      </c>
+      <c r="AT19" s="29">
+        <v>14</v>
+      </c>
       <c r="AU19" s="29"/>
       <c r="AV19" s="29"/>
       <c r="AW19" s="29"/>
@@ -22239,7 +22283,7 @@
       <c r="AZ19" s="29"/>
       <c r="BA19" s="24">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BG19" s="20"/>
       <c r="BH19" s="27" t="s">
@@ -22677,10 +22721,12 @@
       <c r="AQ20" s="30"/>
       <c r="AR20" s="30"/>
       <c r="AS20" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AT20" s="30"/>
+        <f>SUM(AL20:AR20)</f>
+        <v>0</v>
+      </c>
+      <c r="AT20" s="30">
+        <v>130</v>
+      </c>
       <c r="AU20" s="30"/>
       <c r="AV20" s="30"/>
       <c r="AW20" s="30"/>
@@ -22689,7 +22735,7 @@
       <c r="AZ20" s="30"/>
       <c r="BA20" s="24">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="BG20" s="20"/>
       <c r="BH20" s="28" t="s">

</xml_diff>